<commit_message>
new testcase zip download
</commit_message>
<xml_diff>
--- a/TestData/Testexcel.xlsx
+++ b/TestData/Testexcel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27860" windowHeight="12420" firstSheet="22" activeTab="27"/>
+    <workbookView windowWidth="27440" windowHeight="12420" firstSheet="25" activeTab="28"/>
   </bookViews>
   <sheets>
     <sheet name="Testcases" sheetId="1" r:id="rId1"/>
@@ -35,6 +35,7 @@
     <sheet name="CreateDesign" sheetId="26" r:id="rId26"/>
     <sheet name="EditDesign" sheetId="27" r:id="rId27"/>
     <sheet name="DeleteSingleRecord" sheetId="28" r:id="rId28"/>
+    <sheet name="NewDownloadpdfwithoutbckgndzip" sheetId="29" r:id="rId29"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -54,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="82">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -89,7 +90,7 @@
     <t>CreateRecord</t>
   </si>
   <si>
-    <t>18/02/2025 02:00 pm</t>
+    <t>27/02/2025 10:14 am</t>
   </si>
   <si>
     <t>CreateSpace</t>
@@ -173,7 +174,7 @@
     <t>ReshareRecord</t>
   </si>
   <si>
-    <t>16/12/2024 11:51 am</t>
+    <t>04/03/2025 12:31 pm</t>
   </si>
   <si>
     <t>BulkEdit</t>
@@ -212,6 +213,12 @@
     <t>17/02/2025 06:09 pm</t>
   </si>
   <si>
+    <t>DeleteSingleRecord</t>
+  </si>
+  <si>
+    <t>04/03/2025 12:24 pm</t>
+  </si>
+  <si>
     <t>email</t>
   </si>
   <si>
@@ -281,61 +288,19 @@
     <t>Newreg</t>
   </si>
   <si>
-    <t>DeleteSingleRecord</t>
-  </si>
-  <si>
-    <t>24/02/2025 04:49 pm</t>
-  </si>
-  <si>
-    <t>24/02/2025 04:52 pm</t>
-  </si>
-  <si>
-    <t>25/02/2025 12:49 pm</t>
-  </si>
-  <si>
-    <t>25/02/2025 12:51 pm</t>
-  </si>
-  <si>
-    <t>27/02/2025 10:14 am</t>
-  </si>
-  <si>
-    <t>04/03/2025 12:24 pm</t>
-  </si>
-  <si>
-    <t>04/03/2025 12:31 pm</t>
-  </si>
-  <si>
-    <t>04/03/2025 01:57 pm</t>
-  </si>
-  <si>
-    <t>04/03/2025 01:58 pm</t>
-  </si>
-  <si>
-    <t>Archiveregistry</t>
-  </si>
-  <si>
-    <t>04/03/2025 02:01 pm</t>
-  </si>
-  <si>
-    <t>04/03/2025 02:40 pm</t>
-  </si>
-  <si>
-    <t>04/03/2025 02:41 pm</t>
-  </si>
-  <si>
-    <t>04/03/2025 02:43 pm</t>
-  </si>
-  <si>
-    <t>05/03/2025 01:09 pm</t>
-  </si>
-  <si>
-    <t>05/03/2025 02:29 pm</t>
-  </si>
-  <si>
-    <t>05/03/2025 02:32 pm</t>
-  </si>
-  <si>
-    <t>05/03/2025 02:36 pm</t>
+    <t>NewDownloadpdfwithoutbckgndzip</t>
+  </si>
+  <si>
+    <t>06/03/2025 02:11 pm</t>
+  </si>
+  <si>
+    <t>06/03/2025 02:12 pm</t>
+  </si>
+  <si>
+    <t>06/03/2025 02:13 pm</t>
+  </si>
+  <si>
+    <t>06/03/2025 02:15 pm</t>
   </si>
 </sst>
 </file>
@@ -348,7 +313,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -404,13 +369,6 @@
       <color rgb="FF000000"/>
       <name val="Helvetica Neue"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -860,148 +818,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1437,7 +1395,7 @@
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="2" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>7</v>
@@ -1461,7 +1419,7 @@
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="2" t="s">
-        <v>80</v>
+        <v>11</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>7</v>
@@ -1528,7 +1486,7 @@
         <v>22</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>93</v>
+        <v>23</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>7</v>
@@ -1616,7 +1574,7 @@
         <v>38</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>82</v>
+        <v>39</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>7</v>
@@ -1641,7 +1599,7 @@
         <v>43</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>84</v>
+        <v>6</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>7</v>
@@ -1655,7 +1613,7 @@
         <v>44</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>88</v>
+        <v>45</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>7</v>
@@ -1697,23 +1655,23 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" t="s" s="4">
-        <v>75</v>
-      </c>
-      <c r="C25" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="D25" t="s" s="2">
+    <row r="25" spans="1:4">
+      <c r="A25" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="4">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C26" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="D26" t="s" s="2">
         <v>7</v>
@@ -1744,18 +1702,18 @@
   <sheetData>
     <row r="1" ht="18.75" customHeight="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" ht="18.75" customHeight="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1783,18 +1741,18 @@
   <sheetData>
     <row r="1" ht="18.75" customHeight="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" ht="18.75" customHeight="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1822,18 +1780,18 @@
   <sheetData>
     <row r="1" ht="18.75" customHeight="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" ht="18.75" customHeight="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1861,18 +1819,18 @@
   <sheetData>
     <row r="1" ht="18.75" customHeight="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" ht="18.75" customHeight="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1900,18 +1858,18 @@
   <sheetData>
     <row r="1" ht="18.75" customHeight="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" ht="18.75" customHeight="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1939,18 +1897,18 @@
   <sheetData>
     <row r="1" ht="18.75" customHeight="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" ht="18.75" customHeight="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1978,18 +1936,18 @@
   <sheetData>
     <row r="1" ht="18.75" customHeight="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" ht="18.75" customHeight="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -2016,12 +1974,12 @@
   <sheetData>
     <row r="1" ht="18" customHeight="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" ht="18" customHeight="1" spans="1:1">
       <c r="A2" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -2038,7 +1996,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A2" sqref="$A1:$XFD1 $A2:$XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -2049,18 +2007,18 @@
   <sheetData>
     <row r="1" ht="18.75" customHeight="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" ht="18.75" customHeight="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -2088,18 +2046,18 @@
   <sheetData>
     <row r="1" ht="18.75" customHeight="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" ht="18.75" customHeight="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -2127,13 +2085,13 @@
   <sheetData>
     <row r="1" ht="18" customHeight="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B1" s="14"/>
     </row>
     <row r="2" ht="18" customHeight="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B2" s="16"/>
     </row>
@@ -2162,18 +2120,18 @@
   <sheetData>
     <row r="1" ht="18.75" customHeight="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" ht="18.75" customHeight="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -2200,12 +2158,12 @@
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:1">
       <c r="A2" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -2233,18 +2191,18 @@
   <sheetData>
     <row r="1" ht="18.75" customHeight="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" ht="18.75" customHeight="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -2272,18 +2230,18 @@
   <sheetData>
     <row r="1" ht="18.75" customHeight="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" ht="18.75" customHeight="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -2310,12 +2268,12 @@
   <sheetData>
     <row r="1" ht="18.75" customHeight="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" ht="18.75" customHeight="1" spans="1:1">
       <c r="A2" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -2342,12 +2300,12 @@
   <sheetData>
     <row r="1" ht="18.75" customHeight="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" ht="18.75" customHeight="1" spans="1:1">
       <c r="A2" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -2374,12 +2332,12 @@
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:1">
       <c r="A2" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -2406,12 +2364,12 @@
   <sheetData>
     <row r="1" ht="18.75" customHeight="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" ht="18.75" customHeight="1" spans="1:1">
       <c r="A2" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -2425,6 +2383,39 @@
   <sheetPr/>
   <dimension ref="A1:B2"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="$A1:$XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="1" outlineLevelCol="1"/>
+  <sheetData>
+    <row r="1" ht="18.75" customHeight="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" ht="18.75" customHeight="1" spans="1:2">
+      <c r="A2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="$A1:$XFD2"/>
     </sheetView>
@@ -2433,18 +2424,18 @@
   <sheetData>
     <row r="1" ht="18.75" customHeight="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" ht="18.75" customHeight="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -2474,30 +2465,30 @@
   <sheetData>
     <row r="1" ht="18.75" customHeight="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" ht="18.75" customHeight="1" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -2527,28 +2518,28 @@
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:4">
       <c r="A1" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B2" s="15"/>
       <c r="C2" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -2579,36 +2570,36 @@
   <sheetData>
     <row r="1" ht="18.75" customHeight="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" ht="18.75" customHeight="1" spans="1:5">
       <c r="A2" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -2636,18 +2627,18 @@
   <sheetData>
     <row r="1" ht="18.75" customHeight="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" ht="18.75" customHeight="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -2675,18 +2666,18 @@
   <sheetData>
     <row r="1" ht="18.75" customHeight="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" ht="18.75" customHeight="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -2714,18 +2705,18 @@
   <sheetData>
     <row r="1" ht="18.75" customHeight="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" ht="18.75" customHeight="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -2755,36 +2746,36 @@
   <sheetData>
     <row r="1" ht="18.75" customHeight="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" ht="18.75" customHeight="1" spans="1:5">
       <c r="A2" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>